<commit_message>
added crud for lecturers and programmes
</commit_message>
<xml_diff>
--- a/Team Projects Progress.xlsx
+++ b/Team Projects Progress.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="7200" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>View, add, edit and delete requests made by that timetabler</t>
   </si>
@@ -206,9 +206,6 @@
     <t>validation required</t>
   </si>
   <si>
-    <t>This will probably be done with action links</t>
-  </si>
-  <si>
     <t>limit the size of the input maybe?</t>
   </si>
   <si>
@@ -216,6 +213,18 @@
   </si>
   <si>
     <t>Could implement hide/show to hide unpopular facilities</t>
+  </si>
+  <si>
+    <t>multiple "Any room in park/building" rooms cannot be added. Not sure how to get around thing as it’s a problem with adding it to the database</t>
+  </si>
+  <si>
+    <t>multiple "any room in park/building" not working</t>
+  </si>
+  <si>
+    <t>This will probably be done with action links and [Authorize] tags</t>
+  </si>
+  <si>
+    <t>in request, all fields have default values</t>
   </si>
 </sst>
 </file>
@@ -595,8 +604,8 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -647,13 +656,13 @@
         <v>42096</v>
       </c>
       <c r="D3" s="7">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="F3" t="s">
         <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -705,7 +714,7 @@
         <v>42096</v>
       </c>
       <c r="D8" s="7">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F8" t="s">
         <v>52</v>
@@ -852,13 +861,13 @@
         <v>42096</v>
       </c>
       <c r="D22" s="7">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="F22" t="s">
         <v>52</v>
       </c>
       <c r="G22" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -878,7 +887,7 @@
         <v>52</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -906,7 +915,7 @@
         <v>42110</v>
       </c>
       <c r="C25" s="3">
-        <v>42202</v>
+        <v>42111</v>
       </c>
       <c r="D25" s="7">
         <v>1</v>
@@ -950,7 +959,7 @@
         <v>52</v>
       </c>
       <c r="G28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1004,7 +1013,7 @@
         <v>52</v>
       </c>
       <c r="G31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="2" customFormat="1" ht="17.25" thickBot="1">
@@ -1025,7 +1034,7 @@
         <v>52</v>
       </c>
       <c r="G33" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1205,9 +1214,14 @@
       <c r="A50" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="3"/>
+      <c r="B50" s="3">
+        <v>42106</v>
+      </c>
       <c r="D50" s="7">
-        <v>0</v>
+        <v>0.6</v>
+      </c>
+      <c r="G50" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:7">

</xml_diff>

<commit_message>
downgraded EF to 4.0 and lots of functionality
admin allocation stuff, blahblahblah
</commit_message>
<xml_diff>
--- a/Team Projects Progress.xlsx
+++ b/Team Projects Progress.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prakash\Desktop\Work\D3\TeamProject\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="7200" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
   <si>
     <t>View, add, edit and delete requests made by that timetabler</t>
   </si>
@@ -35,9 +30,6 @@
     <t>View requests that have been sent back by the central admin and edit/resubmit as required.</t>
   </si>
   <si>
-    <t>Should be able to sort/filter requests by appropriate fields</t>
-  </si>
-  <si>
     <t>View last year’s requests and edit/resubmit as required.</t>
   </si>
   <si>
@@ -194,18 +186,12 @@
     <t>Scaffolded, i/o needs to be improved (colours for statuses)</t>
   </si>
   <si>
-    <t>Scaffolded but main functionality complete, improve i/o</t>
-  </si>
-  <si>
     <t>Scaffolded, i/o needs to be improved and cannot edit facilities of a room</t>
   </si>
   <si>
     <t>This is simple enough to do using the [Authorize] tag</t>
   </si>
   <si>
-    <t>validation required</t>
-  </si>
-  <si>
     <t>limit the size of the input maybe?</t>
   </si>
   <si>
@@ -218,20 +204,23 @@
     <t>multiple "Any room in park/building" rooms cannot be added. Not sure how to get around thing as it’s a problem with adding it to the database</t>
   </si>
   <si>
-    <t>multiple "any room in park/building" not working</t>
-  </si>
-  <si>
     <t>This will probably be done with action links and [Authorize] tags</t>
   </si>
   <si>
     <t>in request, all fields have default values</t>
+  </si>
+  <si>
+    <t>Dan</t>
+  </si>
+  <si>
+    <t>requestId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,7 +582,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -601,155 +590,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="98.75" customWidth="1"/>
+    <col min="1" max="1" width="98.7109375" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25" thickBot="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="18" thickTop="1" thickBot="1">
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickTop="1">
+    <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3">
         <v>42096</v>
       </c>
+      <c r="C3" s="3">
+        <v>42126</v>
+      </c>
       <c r="D3" s="7">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>42121</v>
+      </c>
+      <c r="C4" s="3">
+        <v>42126</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="D4" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3">
         <v>42096</v>
       </c>
+      <c r="C5" s="3">
+        <v>42129</v>
+      </c>
       <c r="D5" s="7">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="D6" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A7" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3">
+        <v>42096</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>42121</v>
+      </c>
+      <c r="C8" s="3">
+        <v>42126</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3">
+        <v>42096</v>
+      </c>
+      <c r="C9" s="3">
+        <v>42126</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickTop="1">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="3">
-        <v>42096</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="F8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="D9" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3">
-        <v>42096</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="F10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -758,488 +772,507 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickTop="1">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3"/>
       <c r="D13" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="B14" s="3">
+        <v>42122</v>
+      </c>
+      <c r="C14" s="3">
+        <v>42122</v>
+      </c>
       <c r="D14" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="B15" s="3">
+        <v>42123</v>
+      </c>
+      <c r="C15" s="3">
+        <v>42123</v>
+      </c>
       <c r="D15" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B16" s="3"/>
       <c r="D16" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="B17" s="3">
+        <v>42090</v>
+      </c>
+      <c r="C17" s="3">
+        <v>42121</v>
+      </c>
       <c r="D17" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="B18" s="3">
+        <v>42121</v>
+      </c>
       <c r="D18" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="B19" s="3">
+        <v>42096</v>
+      </c>
+      <c r="C19" s="3">
+        <v>42126</v>
+      </c>
       <c r="D19" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
+        <v>42107</v>
+      </c>
+      <c r="C20" s="3">
+        <v>42109</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="3">
+        <v>42110</v>
+      </c>
+      <c r="C21" s="3">
+        <v>42111</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="3">
+        <v>42110</v>
+      </c>
+      <c r="C22" s="3">
+        <v>42111</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="D23" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="D24" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="3">
+        <v>42106</v>
+      </c>
+      <c r="C25" s="3">
+        <v>42109</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="3">
+        <v>42106</v>
+      </c>
+      <c r="C26" s="3">
+        <v>42107</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="3">
+        <v>42096</v>
+      </c>
+      <c r="C27" s="3">
+        <v>42109</v>
+      </c>
+      <c r="D27" s="7">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="3">
+        <v>42096</v>
+      </c>
+      <c r="C28" s="3">
+        <v>42108</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="D30" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="3">
         <v>42090</v>
       </c>
-      <c r="D20" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="F20" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="D21" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="3">
-        <v>42096</v>
-      </c>
-      <c r="D22" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="F22" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="3">
-        <v>42107</v>
-      </c>
-      <c r="C23" s="3">
-        <v>42109</v>
-      </c>
-      <c r="D23" s="7">
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="3">
-        <v>42110</v>
-      </c>
-      <c r="C24" s="3">
-        <v>42111</v>
-      </c>
-      <c r="D24" s="7">
-        <v>1</v>
-      </c>
-      <c r="F24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="3">
-        <v>42110</v>
-      </c>
-      <c r="C25" s="3">
-        <v>42111</v>
-      </c>
-      <c r="D25" s="7">
-        <v>1</v>
-      </c>
-      <c r="F25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="D26" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="D27" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="3">
-        <v>42106</v>
-      </c>
-      <c r="C28" s="3">
-        <v>42109</v>
-      </c>
-      <c r="D28" s="7">
-        <v>1</v>
-      </c>
-      <c r="F28" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="3">
-        <v>42106</v>
-      </c>
-      <c r="C29" s="3">
-        <v>42107</v>
-      </c>
-      <c r="D29" s="7">
-        <v>1</v>
-      </c>
-      <c r="F29" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="3">
-        <v>42096</v>
-      </c>
-      <c r="C30" s="3">
-        <v>42109</v>
-      </c>
-      <c r="D30" s="7">
-        <v>1</v>
-      </c>
-      <c r="F30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="3">
-        <v>42096</v>
-      </c>
       <c r="C31" s="3">
-        <v>42108</v>
+        <v>42118</v>
       </c>
       <c r="D31" s="7">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="2" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A32" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" ht="15" thickTop="1">
+      <c r="B32" s="3">
+        <v>42090</v>
+      </c>
+      <c r="C32" s="3">
+        <v>42118</v>
+      </c>
+      <c r="D32" s="7">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="B33" s="3">
+        <v>42125</v>
+      </c>
+      <c r="C33" s="3">
+        <v>42125</v>
+      </c>
       <c r="D33" s="7">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>52</v>
-      </c>
-      <c r="G33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B34" s="3">
-        <v>42090</v>
+        <v>42125</v>
+      </c>
+      <c r="C34" s="3">
+        <v>42125</v>
       </c>
       <c r="D34" s="7">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>52</v>
-      </c>
-      <c r="G34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B35" s="3">
         <v>42090</v>
       </c>
+      <c r="C35" s="3">
+        <v>42096</v>
+      </c>
       <c r="D35" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>52</v>
-      </c>
-      <c r="G35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="3"/>
-      <c r="D36" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="B37" s="3">
+        <v>42090</v>
+      </c>
       <c r="D37" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>0.6</v>
+      </c>
+      <c r="F37" t="s">
+        <v>51</v>
+      </c>
+      <c r="G37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="3">
-        <v>42090</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B38" s="3"/>
       <c r="D38" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="F38" t="s">
-        <v>52</v>
-      </c>
-      <c r="G38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="2" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A39" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:7" ht="15" thickTop="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="D39" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="3">
-        <v>42090</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B40" s="3"/>
       <c r="D40" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="F40" t="s">
-        <v>52</v>
-      </c>
-      <c r="G40" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B41" s="3"/>
       <c r="D41" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B42" s="3"/>
       <c r="D42" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B43" s="3"/>
       <c r="D43" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B44" s="3"/>
       <c r="D44" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B45" s="3"/>
       <c r="D45" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B46" s="3"/>
       <c r="D46" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="B47" s="3">
+        <v>42106</v>
+      </c>
       <c r="D47" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>0.6</v>
+      </c>
+      <c r="F47" t="s">
+        <v>51</v>
+      </c>
+      <c r="G47" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="B48" s="3">
+        <v>42088</v>
+      </c>
+      <c r="C48" s="3"/>
       <c r="D48" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49" s="3"/>
-      <c r="D49" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="3">
-        <v>42106</v>
-      </c>
-      <c r="D50" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="G50" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" s="3">
-        <v>42088</v>
-      </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="7">
         <v>0.95</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F48" t="s">
+        <v>51</v>
+      </c>
+      <c r="G48" t="s">
         <v>52</v>
-      </c>
-      <c r="G51" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alex Up to date
</commit_message>
<xml_diff>
--- a/Team Projects Progress.xlsx
+++ b/Team Projects Progress.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prakash\Desktop\Work\D3\TeamProject\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="7200" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
   <si>
     <t>View, add, edit and delete requests made by that timetabler</t>
   </si>
@@ -35,9 +30,6 @@
     <t>View requests that have been sent back by the central admin and edit/resubmit as required.</t>
   </si>
   <si>
-    <t>Should be able to sort/filter requests by appropriate fields</t>
-  </si>
-  <si>
     <t>View last year’s requests and edit/resubmit as required.</t>
   </si>
   <si>
@@ -194,21 +186,12 @@
     <t>Scaffolded, i/o needs to be improved (colours for statuses)</t>
   </si>
   <si>
-    <t>Scaffolded but main functionality complete, improve i/o</t>
-  </si>
-  <si>
     <t>Scaffolded, i/o needs to be improved and cannot edit facilities of a room</t>
   </si>
   <si>
     <t>This is simple enough to do using the [Authorize] tag</t>
   </si>
   <si>
-    <t>validation required</t>
-  </si>
-  <si>
-    <t>This will probably be done with action links</t>
-  </si>
-  <si>
     <t>limit the size of the input maybe?</t>
   </si>
   <si>
@@ -216,13 +199,28 @@
   </si>
   <si>
     <t>Could implement hide/show to hide unpopular facilities</t>
+  </si>
+  <si>
+    <t>multiple "Any room in park/building" rooms cannot be added. Not sure how to get around thing as it’s a problem with adding it to the database</t>
+  </si>
+  <si>
+    <t>This will probably be done with action links and [Authorize] tags</t>
+  </si>
+  <si>
+    <t>in request, all fields have default values</t>
+  </si>
+  <si>
+    <t>Dan</t>
+  </si>
+  <si>
+    <t>requestId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -584,7 +582,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -592,155 +590,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="98.75" customWidth="1"/>
+    <col min="1" max="1" width="98.7109375" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25" thickBot="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="18" thickTop="1" thickBot="1">
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickTop="1">
+    <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3">
         <v>42096</v>
       </c>
+      <c r="C3" s="3">
+        <v>42126</v>
+      </c>
       <c r="D3" s="7">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3">
+        <v>42121</v>
+      </c>
+      <c r="C4" s="3">
+        <v>42126</v>
+      </c>
       <c r="D4" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>0.9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3">
         <v>42096</v>
       </c>
+      <c r="C5" s="3">
+        <v>42129</v>
+      </c>
       <c r="D5" s="7">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="D6" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A7" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3">
+        <v>42096</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>42121</v>
+      </c>
+      <c r="C8" s="3">
+        <v>42126</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3">
+        <v>42096</v>
+      </c>
+      <c r="C9" s="3">
+        <v>42126</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickTop="1">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="3">
-        <v>42096</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="D9" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3">
-        <v>42096</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="F10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -749,483 +772,507 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickTop="1">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3"/>
       <c r="D13" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="B14" s="3">
+        <v>42122</v>
+      </c>
+      <c r="C14" s="3">
+        <v>42122</v>
+      </c>
       <c r="D14" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="B15" s="3">
+        <v>42123</v>
+      </c>
+      <c r="C15" s="3">
+        <v>42123</v>
+      </c>
       <c r="D15" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B16" s="3"/>
       <c r="D16" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="B17" s="3">
+        <v>42090</v>
+      </c>
+      <c r="C17" s="3">
+        <v>42121</v>
+      </c>
       <c r="D17" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="B18" s="3">
+        <v>42121</v>
+      </c>
       <c r="D18" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="B19" s="3">
+        <v>42096</v>
+      </c>
+      <c r="C19" s="3">
+        <v>42126</v>
+      </c>
       <c r="D19" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
+        <v>42107</v>
+      </c>
+      <c r="C20" s="3">
+        <v>42109</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="3">
+        <v>42110</v>
+      </c>
+      <c r="C21" s="3">
+        <v>42111</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="3">
+        <v>42110</v>
+      </c>
+      <c r="C22" s="3">
+        <v>42111</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="D23" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="D24" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="3">
+        <v>42106</v>
+      </c>
+      <c r="C25" s="3">
+        <v>42109</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="3">
+        <v>42106</v>
+      </c>
+      <c r="C26" s="3">
+        <v>42107</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="3">
+        <v>42096</v>
+      </c>
+      <c r="C27" s="3">
+        <v>42109</v>
+      </c>
+      <c r="D27" s="7">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="3">
+        <v>42096</v>
+      </c>
+      <c r="C28" s="3">
+        <v>42108</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="D30" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="3">
         <v>42090</v>
       </c>
-      <c r="D20" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="F20" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="D21" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="3">
-        <v>42096</v>
-      </c>
-      <c r="D22" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="F22" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="3">
-        <v>42107</v>
-      </c>
-      <c r="C23" s="3">
-        <v>42109</v>
-      </c>
-      <c r="D23" s="7">
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="3">
-        <v>42110</v>
-      </c>
-      <c r="C24" s="3">
-        <v>42111</v>
-      </c>
-      <c r="D24" s="7">
-        <v>1</v>
-      </c>
-      <c r="F24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="3">
-        <v>42110</v>
-      </c>
-      <c r="C25" s="3">
-        <v>42202</v>
-      </c>
-      <c r="D25" s="7">
-        <v>1</v>
-      </c>
-      <c r="F25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="D26" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="D27" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="3">
-        <v>42106</v>
-      </c>
-      <c r="C28" s="3">
-        <v>42109</v>
-      </c>
-      <c r="D28" s="7">
-        <v>1</v>
-      </c>
-      <c r="F28" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="3">
-        <v>42106</v>
-      </c>
-      <c r="C29" s="3">
-        <v>42107</v>
-      </c>
-      <c r="D29" s="7">
-        <v>1</v>
-      </c>
-      <c r="F29" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="3">
-        <v>42096</v>
-      </c>
-      <c r="C30" s="3">
-        <v>42109</v>
-      </c>
-      <c r="D30" s="7">
-        <v>1</v>
-      </c>
-      <c r="F30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="3">
-        <v>42096</v>
-      </c>
       <c r="C31" s="3">
-        <v>42108</v>
+        <v>42118</v>
       </c>
       <c r="D31" s="7">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G31" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="2" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A32" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" ht="15" thickTop="1">
+      <c r="B32" s="3">
+        <v>42090</v>
+      </c>
+      <c r="C32" s="3">
+        <v>42118</v>
+      </c>
+      <c r="D32" s="7">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="B33" s="3">
+        <v>42125</v>
+      </c>
+      <c r="C33" s="3">
+        <v>42125</v>
+      </c>
       <c r="D33" s="7">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>52</v>
-      </c>
-      <c r="G33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B34" s="3">
-        <v>42090</v>
+        <v>42125</v>
+      </c>
+      <c r="C34" s="3">
+        <v>42125</v>
       </c>
       <c r="D34" s="7">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>52</v>
-      </c>
-      <c r="G34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B35" s="3">
         <v>42090</v>
       </c>
+      <c r="C35" s="3">
+        <v>42096</v>
+      </c>
       <c r="D35" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>52</v>
-      </c>
-      <c r="G35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="3"/>
-      <c r="D36" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="B37" s="3">
+        <v>42090</v>
+      </c>
       <c r="D37" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>0.6</v>
+      </c>
+      <c r="F37" t="s">
+        <v>51</v>
+      </c>
+      <c r="G37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="3">
-        <v>42090</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B38" s="3"/>
       <c r="D38" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="F38" t="s">
-        <v>52</v>
-      </c>
-      <c r="G38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="2" customFormat="1" ht="17.25" thickBot="1">
-      <c r="A39" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:7" ht="15" thickTop="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="D39" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="3">
-        <v>42090</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B40" s="3"/>
       <c r="D40" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="F40" t="s">
-        <v>52</v>
-      </c>
-      <c r="G40" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B41" s="3"/>
       <c r="D41" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B42" s="3"/>
       <c r="D42" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B43" s="3"/>
       <c r="D43" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B44" s="3"/>
       <c r="D44" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B45" s="3"/>
       <c r="D45" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B46" s="3"/>
       <c r="D46" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="B47" s="3">
+        <v>42106</v>
+      </c>
       <c r="D47" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>0.6</v>
+      </c>
+      <c r="F47" t="s">
+        <v>51</v>
+      </c>
+      <c r="G47" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="B48" s="3">
+        <v>42088</v>
+      </c>
+      <c r="C48" s="3"/>
       <c r="D48" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49" s="3"/>
-      <c r="D49" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="3"/>
-      <c r="D50" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" s="3">
-        <v>42088</v>
-      </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="7">
         <v>0.95</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F48" t="s">
+        <v>51</v>
+      </c>
+      <c r="G48" t="s">
         <v>52</v>
-      </c>
-      <c r="G51" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>